<commit_message>
Opciones para actualizar registro especifico. (Author o Price)
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ficheros-Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\grupo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A946DC7-FE17-4E37-B79A-F4FCFF9518E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="8625" windowWidth="12210" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Java Books" r:id="rId1" sheetId="1"/>
+    <sheet name="Java Books" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -101,8 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,16 +130,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -156,10 +156,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -194,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,7 +229,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,21 +323,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -354,7 +354,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -406,27 +406,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -454,7 +454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,7 +468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -482,7 +482,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -496,7 +496,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -510,7 +510,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -524,9 +524,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7.0</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -534,13 +534,13 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="n">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8.0</v>
+      <c r="D8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -548,13 +548,13 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="n">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
+      <c r="D9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -562,13 +562,13 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" t="n">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10.0</v>
+      <c r="D10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -576,11 +576,11 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="n">
-        <v>41.0</v>
+      <c r="D11">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modificación en menu de actualización y creación de función para actualizar registros según un id.
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\grupo1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A946DC7-FE17-4E37-B79A-F4FCFF9518E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B972E0-8D7D-4ABE-B96C-4D5B17F29606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Juan Stand</t>
   </si>
   <si>
-    <t>Luisa Pedroza</t>
-  </si>
-  <si>
     <t>Ana Matia Mujica</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>Luisa Pedraza</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:D15"/>
     </sheetView>
   </sheetViews>
@@ -462,7 +462,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>78</v>
@@ -490,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>102</v>
@@ -504,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>52</v>
@@ -518,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>500</v>
@@ -529,10 +529,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8">
         <v>16</v>
@@ -543,10 +543,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
       <c r="D9">
         <v>26</v>
@@ -557,10 +557,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
       <c r="D10">
         <v>32</v>
@@ -571,10 +571,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11">
         <v>41</v>

</xml_diff>